<commit_message>
update today actual hours
</commit_message>
<xml_diff>
--- a/14.01-01.02.xlsx
+++ b/14.01-01.02.xlsx
@@ -23,6 +23,40 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Anna Sharuntsova.EXT</author>
+  </authors>
+  <commentList>
+    <comment ref="J6" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Anna Sharuntsova.EXT:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+с вычетом 1,5 на английский</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="3">
   <si>
@@ -39,7 +73,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -78,6 +112,19 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="204"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="7">
@@ -452,11 +499,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:M31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3:M4"/>
+      <selection activeCell="L6" sqref="L6:L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -556,17 +603,21 @@
       <c r="E6" s="1">
         <v>0.5</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="10">
         <v>5</v>
       </c>
       <c r="G6" s="1">
         <v>0.51388888888888895</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="10">
         <v>7</v>
       </c>
-      <c r="I6" s="1"/>
-      <c r="J6" s="8"/>
+      <c r="I6" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="J6" s="8">
+        <v>6</v>
+      </c>
       <c r="K6" s="1"/>
       <c r="L6" s="8"/>
       <c r="M6" s="7"/>
@@ -578,12 +629,14 @@
       <c r="E7" s="1">
         <v>0.70833333333333337</v>
       </c>
-      <c r="F7" s="6"/>
+      <c r="F7" s="10"/>
       <c r="G7" s="1">
         <v>0.80555555555555547</v>
       </c>
-      <c r="H7" s="6"/>
-      <c r="I7" s="1"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="1">
+        <v>0.8125</v>
+      </c>
       <c r="J7" s="8"/>
       <c r="K7" s="1"/>
       <c r="L7" s="8"/>
@@ -816,6 +869,48 @@
     </row>
   </sheetData>
   <mergeCells count="56">
+    <mergeCell ref="J27:J28"/>
+    <mergeCell ref="L27:L28"/>
+    <mergeCell ref="M27:M28"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="F30:F31"/>
+    <mergeCell ref="H30:H31"/>
+    <mergeCell ref="J30:J31"/>
+    <mergeCell ref="L30:L31"/>
+    <mergeCell ref="M30:M31"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="H27:H28"/>
+    <mergeCell ref="L11:L12"/>
+    <mergeCell ref="M11:M12"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="J14:J15"/>
+    <mergeCell ref="L14:L15"/>
+    <mergeCell ref="M14:M15"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="L6:L7"/>
+    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="M3:M4"/>
     <mergeCell ref="L19:L20"/>
     <mergeCell ref="M19:M20"/>
     <mergeCell ref="B22:B23"/>
@@ -830,50 +925,9 @@
     <mergeCell ref="F19:F20"/>
     <mergeCell ref="H19:H20"/>
     <mergeCell ref="J19:J20"/>
-    <mergeCell ref="L6:L7"/>
-    <mergeCell ref="M6:M7"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="L3:L4"/>
-    <mergeCell ref="J3:J4"/>
-    <mergeCell ref="M3:M4"/>
-    <mergeCell ref="L11:L12"/>
-    <mergeCell ref="M11:M12"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="J14:J15"/>
-    <mergeCell ref="L14:L15"/>
-    <mergeCell ref="M14:M15"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="J27:J28"/>
-    <mergeCell ref="L27:L28"/>
-    <mergeCell ref="M27:M28"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="F30:F31"/>
-    <mergeCell ref="H30:H31"/>
-    <mergeCell ref="J30:J31"/>
-    <mergeCell ref="L30:L31"/>
-    <mergeCell ref="M30:M31"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="F27:F28"/>
-    <mergeCell ref="H27:H28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
set today actual time
</commit_message>
<xml_diff>
--- a/14.01-01.02.xlsx
+++ b/14.01-01.02.xlsx
@@ -455,8 +455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6:J7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -571,9 +571,15 @@
       <c r="J6" s="8">
         <v>6.5</v>
       </c>
-      <c r="K6" s="1"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="7"/>
+      <c r="K6" s="1">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="L6" s="8">
+        <v>6.5</v>
+      </c>
+      <c r="M6" s="7">
+        <v>25</v>
+      </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7" s="8"/>
@@ -591,7 +597,9 @@
         <v>0.77083333333333337</v>
       </c>
       <c r="J7" s="8"/>
-      <c r="K7" s="1"/>
+      <c r="K7" s="1">
+        <v>0.75</v>
+      </c>
       <c r="L7" s="8"/>
       <c r="M7" s="7"/>
     </row>
@@ -822,6 +830,48 @@
     </row>
   </sheetData>
   <mergeCells count="56">
+    <mergeCell ref="J27:J28"/>
+    <mergeCell ref="L27:L28"/>
+    <mergeCell ref="M27:M28"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="F30:F31"/>
+    <mergeCell ref="H30:H31"/>
+    <mergeCell ref="J30:J31"/>
+    <mergeCell ref="L30:L31"/>
+    <mergeCell ref="M30:M31"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="H27:H28"/>
+    <mergeCell ref="L11:L12"/>
+    <mergeCell ref="M11:M12"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="J14:J15"/>
+    <mergeCell ref="L14:L15"/>
+    <mergeCell ref="M14:M15"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="L6:L7"/>
+    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="M3:M4"/>
     <mergeCell ref="L19:L20"/>
     <mergeCell ref="M19:M20"/>
     <mergeCell ref="B22:B23"/>
@@ -836,48 +886,6 @@
     <mergeCell ref="F19:F20"/>
     <mergeCell ref="H19:H20"/>
     <mergeCell ref="J19:J20"/>
-    <mergeCell ref="L6:L7"/>
-    <mergeCell ref="M6:M7"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="L3:L4"/>
-    <mergeCell ref="J3:J4"/>
-    <mergeCell ref="M3:M4"/>
-    <mergeCell ref="L11:L12"/>
-    <mergeCell ref="M11:M12"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="J14:J15"/>
-    <mergeCell ref="L14:L15"/>
-    <mergeCell ref="M14:M15"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="J27:J28"/>
-    <mergeCell ref="L27:L28"/>
-    <mergeCell ref="M27:M28"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="F30:F31"/>
-    <mergeCell ref="H30:H31"/>
-    <mergeCell ref="J30:J31"/>
-    <mergeCell ref="L30:L31"/>
-    <mergeCell ref="M30:M31"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="F27:F28"/>
-    <mergeCell ref="H27:H28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update intended time and actual today
</commit_message>
<xml_diff>
--- a/14.01-01.02.xlsx
+++ b/14.01-01.02.xlsx
@@ -455,8 +455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -604,15 +604,25 @@
       <c r="M7" s="7"/>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="C10" s="2"/>
+      <c r="C10" s="2">
+        <v>43486</v>
+      </c>
       <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
+      <c r="E10" s="2">
+        <v>43487</v>
+      </c>
       <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
+      <c r="G10" s="2">
+        <v>43488</v>
+      </c>
       <c r="H10" s="3"/>
-      <c r="I10" s="2"/>
+      <c r="I10" s="2">
+        <v>43489</v>
+      </c>
       <c r="J10" s="3"/>
-      <c r="K10" s="2"/>
+      <c r="K10" s="2">
+        <v>43490</v>
+      </c>
       <c r="L10" s="3"/>
       <c r="M10" s="4" t="s">
         <v>0</v>
@@ -623,13 +633,27 @@
         <v>1</v>
       </c>
       <c r="C11" s="1"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="6"/>
+      <c r="D11" s="6">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0.46875</v>
+      </c>
+      <c r="F11" s="6">
+        <v>8</v>
+      </c>
+      <c r="G11" s="1">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="H11" s="6">
+        <v>8</v>
+      </c>
+      <c r="I11" s="1">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="J11" s="6">
+        <v>8</v>
+      </c>
       <c r="K11" s="1"/>
       <c r="L11" s="6"/>
       <c r="M11" s="7"/>
@@ -638,11 +662,17 @@
       <c r="B12" s="9"/>
       <c r="C12" s="1"/>
       <c r="D12" s="6"/>
-      <c r="E12" s="1"/>
+      <c r="E12" s="1">
+        <v>0.80208333333333337</v>
+      </c>
       <c r="F12" s="6"/>
-      <c r="G12" s="1"/>
+      <c r="G12" s="1">
+        <v>0.82291666666666663</v>
+      </c>
       <c r="H12" s="6"/>
-      <c r="I12" s="1"/>
+      <c r="I12" s="1">
+        <v>0.76041666666666663</v>
+      </c>
       <c r="J12" s="6"/>
       <c r="K12" s="1"/>
       <c r="L12" s="6"/>
@@ -653,9 +683,15 @@
         <v>2</v>
       </c>
       <c r="C14" s="1"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="8"/>
+      <c r="D14" s="8">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0.46875</v>
+      </c>
+      <c r="F14" s="8">
+        <v>8</v>
+      </c>
       <c r="G14" s="1"/>
       <c r="H14" s="8"/>
       <c r="I14" s="1"/>
@@ -668,7 +704,9 @@
       <c r="B15" s="8"/>
       <c r="C15" s="1"/>
       <c r="D15" s="8"/>
-      <c r="E15" s="1"/>
+      <c r="E15" s="1">
+        <v>0.80208333333333337</v>
+      </c>
       <c r="F15" s="8"/>
       <c r="G15" s="1"/>
       <c r="H15" s="8"/>

</xml_diff>